<commit_message>
add needed data from run.py
</commit_message>
<xml_diff>
--- a/HRX/Test/test_case.xlsx
+++ b/HRX/Test/test_case.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="460" windowWidth="15020" windowHeight="12820" tabRatio="500"/>
+    <workbookView xWindow="120" yWindow="460" windowWidth="15020" windowHeight="14160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6704" uniqueCount="5427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6706" uniqueCount="5428">
   <si>
     <t>node</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -16357,6 +16357,19 @@
     <t>好的</t>
     <rPh sb="0" eb="1">
       <t>hao de</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>我没有钱</t>
+    <rPh sb="0" eb="1">
+      <t>wo</t>
+    </rPh>
+    <rPh sb="1" eb="2">
+      <t>mei you</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>qian</t>
     </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -16730,8 +16743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="C109" sqref="C109"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="D104" sqref="D104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18074,6 +18087,15 @@
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>95</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>5419</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>5427</v>
+      </c>
+      <c r="D96" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>